<commit_message>
fix pdf for 七十迈 (#145)
</commit_message>
<xml_diff>
--- a/src/main/resources/agent_voucher/108#voucher_template.xlsx
+++ b/src/main/resources/agent_voucher/108#voucher_template.xlsx
@@ -347,6 +347,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -400,12 +406,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -607,6 +607,44 @@
         <a:xfrm>
           <a:off x="25400" y="25400"/>
           <a:ext cx="3724835" cy="642680"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>806824</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>16190</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="图片 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="25400" y="25400"/>
+          <a:ext cx="3530600" cy="618319"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -882,7 +920,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15:I15"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -895,35 +933,35 @@
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="17"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A2" s="4"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="15"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A3" s="4"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="15"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="17"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="4"/>
@@ -945,11 +983,11 @@
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="8"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="19"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="21"/>
     </row>
     <row r="6" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="9" t="s">
@@ -960,11 +998,11 @@
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="11"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="21"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="23"/>
     </row>
     <row r="7" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="9" t="s">
@@ -975,11 +1013,11 @@
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="11"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="27"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="29"/>
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A8" s="9" t="s">
@@ -990,11 +1028,11 @@
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="11"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="29"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="31"/>
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A9" s="9" t="s">
@@ -1005,11 +1043,11 @@
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="11"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="27"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="29"/>
     </row>
     <row r="10" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="9" t="s">
@@ -1020,11 +1058,11 @@
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="11"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="25"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="27"/>
     </row>
     <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A11" s="9" t="s">
@@ -1035,11 +1073,11 @@
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="11"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="23"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="25"/>
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A12" s="9" t="s">
@@ -1050,11 +1088,11 @@
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="11"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="21"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="23"/>
     </row>
     <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A13" s="9" t="s">
@@ -1065,11 +1103,11 @@
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="11"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="25"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="27"/>
     </row>
     <row r="14" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="9" t="s">
@@ -1080,11 +1118,11 @@
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="11"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="25"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="27"/>
     </row>
     <row r="15" spans="1:9" ht="134" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="9" t="s">
@@ -1095,11 +1133,11 @@
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="11"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="13"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="15"/>
     </row>
     <row r="16" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="9" t="s">
@@ -1110,22 +1148,22 @@
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="13"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="15"/>
     </row>
     <row r="17" spans="1:9" ht="101" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="30"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="15">

</xml_diff>